<commit_message>
GCI from curves averages
</commit_message>
<xml_diff>
--- a/data/curve_for_gci.xlsx
+++ b/data/curve_for_gci.xlsx
@@ -31,64 +31,64 @@
     <t>x</t>
   </si>
   <si>
-    <t>phi_-1.0000</t>
-  </si>
-  <si>
-    <t>phi_-0.9000</t>
-  </si>
-  <si>
-    <t>phi_-0.8000</t>
-  </si>
-  <si>
-    <t>phi_-0.7000</t>
-  </si>
-  <si>
-    <t>phi_-0.6000</t>
-  </si>
-  <si>
-    <t>phi_-0.5000</t>
-  </si>
-  <si>
-    <t>phi_-0.4000</t>
-  </si>
-  <si>
-    <t>phi_-0.3000</t>
-  </si>
-  <si>
-    <t>phi_-0.2000</t>
-  </si>
-  <si>
-    <t>phi_-0.1000</t>
-  </si>
-  <si>
-    <t>phi_0.0000</t>
+    <t>phi_-0.0000</t>
+  </si>
+  <si>
+    <t>phi_0.0500</t>
   </si>
   <si>
     <t>phi_0.1000</t>
   </si>
   <si>
+    <t>phi_0.1500</t>
+  </si>
+  <si>
     <t>phi_0.2000</t>
   </si>
   <si>
+    <t>phi_0.2500</t>
+  </si>
+  <si>
     <t>phi_0.3000</t>
   </si>
   <si>
+    <t>phi_0.3500</t>
+  </si>
+  <si>
     <t>phi_0.4000</t>
   </si>
   <si>
+    <t>phi_0.4500</t>
+  </si>
+  <si>
     <t>phi_0.5000</t>
   </si>
   <si>
+    <t>phi_0.5500</t>
+  </si>
+  <si>
     <t>phi_0.6000</t>
   </si>
   <si>
+    <t>phi_0.6500</t>
+  </si>
+  <si>
     <t>phi_0.7000</t>
   </si>
   <si>
+    <t>phi_0.7500</t>
+  </si>
+  <si>
     <t>phi_0.8000</t>
   </si>
   <si>
+    <t>phi_0.8500</t>
+  </si>
+  <si>
     <t>phi_0.9000</t>
+  </si>
+  <si>
+    <t>phi_0.9500</t>
   </si>
   <si>
     <t>phi_1.0000</t>
@@ -477,16 +477,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0.0762028</v>
+        <v>0.446113646</v>
       </c>
       <c r="C2">
-        <v>0.098555</v>
+        <v>0.442592859</v>
       </c>
       <c r="D2">
-        <v>0.118094</v>
+        <v>0.4470689</v>
       </c>
       <c r="E2">
-        <v>-1</v>
+        <v>-7.13393092E-07</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -494,16 +494,16 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>0.09082753195903717</v>
+        <v>0.4246112354279316</v>
       </c>
       <c r="C3">
-        <v>0.1069450247067137</v>
+        <v>0.4262847582645582</v>
       </c>
       <c r="D3">
-        <v>0.1103875320142812</v>
+        <v>0.435861379980351</v>
       </c>
       <c r="E3">
-        <v>-0.9</v>
+        <v>0.04999932227656259</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -511,16 +511,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>0.08480150651392439</v>
+        <v>0.362232850563531</v>
       </c>
       <c r="C4">
-        <v>0.09394560705828647</v>
+        <v>0.3635276939148809</v>
       </c>
       <c r="D4">
-        <v>0.09213723277681812</v>
+        <v>0.3698628781433433</v>
       </c>
       <c r="E4">
-        <v>-0.8</v>
+        <v>0.09999935794621718</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -528,16 +528,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>0.07677222379981566</v>
+        <v>0.2869568017485726</v>
       </c>
       <c r="C5">
-        <v>0.07793045418526394</v>
+        <v>0.2929609431107805</v>
       </c>
       <c r="D5">
-        <v>0.07660007303170682</v>
+        <v>0.2979116755464833</v>
       </c>
       <c r="E5">
-        <v>-0.7</v>
+        <v>0.1499993936158718</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -545,16 +545,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>0.06781354697431134</v>
+        <v>0.2085413773140853</v>
       </c>
       <c r="C6">
-        <v>0.06033275318280158</v>
+        <v>0.2167929287941868</v>
       </c>
       <c r="D6">
-        <v>0.06161549486511007</v>
+        <v>0.2201327974124013</v>
       </c>
       <c r="E6">
-        <v>-0.6</v>
+        <v>0.1999994292855264</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -562,16 +562,16 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>0.05830345210737423</v>
+        <v>0.1351285381754221</v>
       </c>
       <c r="C7">
-        <v>0.04100529759006474</v>
+        <v>0.1423025141596007</v>
       </c>
       <c r="D7">
-        <v>0.0501978632914754</v>
+        <v>0.14372573426556</v>
       </c>
       <c r="E7">
-        <v>-0.5</v>
+        <v>0.249999464955181</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -579,16 +579,16 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>0.05075089456044511</v>
+        <v>0.07138259991756449</v>
       </c>
       <c r="C8">
-        <v>0.01698417226446381</v>
+        <v>0.07674601964131285</v>
       </c>
       <c r="D8">
-        <v>0.04546218491543554</v>
+        <v>0.0771815567248072</v>
       </c>
       <c r="E8">
-        <v>-0.3999999999999999</v>
+        <v>0.2999995006248355</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -596,16 +596,16 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>0.04697763717490644</v>
+        <v>0.02297510738591806</v>
       </c>
       <c r="C9">
-        <v>0.01846762777251613</v>
+        <v>0.02629345425254802</v>
       </c>
       <c r="D9">
-        <v>0.04518322001283182</v>
+        <v>0.02552679883793104</v>
       </c>
       <c r="E9">
-        <v>-0.2999999999999999</v>
+        <v>0.3499995362944902</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -613,16 +613,16 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>0.04776815328797625</v>
+        <v>0.04411748410674251</v>
       </c>
       <c r="C10">
-        <v>0.02834420456962991</v>
+        <v>0.04416111023660232</v>
       </c>
       <c r="D10">
-        <v>0.04425208367883684</v>
+        <v>0.03993078715810641</v>
       </c>
       <c r="E10">
-        <v>-0.2</v>
+        <v>0.3999995719641448</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -630,16 +630,16 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>0.05087885814055112</v>
+        <v>0.08988136754102584</v>
       </c>
       <c r="C11">
-        <v>0.03474009492370726</v>
+        <v>0.08991195453941069</v>
       </c>
       <c r="D11">
-        <v>0.0402816269964423</v>
+        <v>0.08629661294338958</v>
       </c>
       <c r="E11">
-        <v>-0.09999999999999998</v>
+        <v>0.4499996076337994</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -647,16 +647,16 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>0.05109250256374864</v>
+        <v>0.1361954070995965</v>
       </c>
       <c r="C12">
-        <v>0.03852522959707071</v>
+        <v>0.1359988540096508</v>
       </c>
       <c r="D12">
-        <v>0.03274868135438866</v>
+        <v>0.1326337387927119</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.499999643303454</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -664,16 +664,16 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>0.04582933606166305</v>
+        <v>0.1840127752610901</v>
       </c>
       <c r="C13">
-        <v>0.03577339444571054</v>
+        <v>0.1821744756461599</v>
       </c>
       <c r="D13">
-        <v>0.03749797716201021</v>
+        <v>0.178864023292082</v>
       </c>
       <c r="E13">
-        <v>0.1000000000000001</v>
+        <v>0.5499996789731085</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -681,16 +681,16 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>0.2120509971738638</v>
+        <v>0.2383783516901995</v>
       </c>
       <c r="C14">
-        <v>0.3131332320201378</v>
+        <v>0.2323943639211221</v>
       </c>
       <c r="D14">
-        <v>0.4508810111691258</v>
+        <v>0.2293526279103272</v>
       </c>
       <c r="E14">
-        <v>0.2000000000000002</v>
+        <v>0.599999714642763</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -698,16 +698,16 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>0.3340436573372461</v>
+        <v>0.3127474316144384</v>
       </c>
       <c r="C15">
-        <v>0.3991256194718149</v>
+        <v>0.2995419889334269</v>
       </c>
       <c r="D15">
-        <v>0.3676637667484861</v>
+        <v>0.2986893882845401</v>
       </c>
       <c r="E15">
-        <v>0.3</v>
+        <v>0.6499997503124176</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -715,16 +715,16 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0.2026699242124337</v>
+        <v>0.4283596859988836</v>
       </c>
       <c r="C16">
-        <v>0.1561133070535207</v>
+        <v>0.4116351294545521</v>
       </c>
       <c r="D16">
-        <v>0.02009066353763644</v>
+        <v>0.4192823897277798</v>
       </c>
       <c r="E16">
-        <v>0.4000000000000001</v>
+        <v>0.6999997859820722</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -732,16 +732,16 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>0.06239887968652123</v>
+        <v>0.6075918816272678</v>
       </c>
       <c r="C17">
-        <v>0.04593695559616863</v>
+        <v>0.5950562549488467</v>
       </c>
       <c r="D17">
-        <v>0.06431953346885186</v>
+        <v>0.6147961707990083</v>
       </c>
       <c r="E17">
-        <v>0.5</v>
+        <v>0.7499998216517269</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -749,16 +749,16 @@
         <v>21</v>
       </c>
       <c r="B18">
-        <v>0.06097875166938957</v>
+        <v>0.8359285424689332</v>
       </c>
       <c r="C18">
-        <v>0.03249835592860255</v>
+        <v>0.8321582760263507</v>
       </c>
       <c r="D18">
-        <v>0.03609276946123521</v>
+        <v>0.8591015965897354</v>
       </c>
       <c r="E18">
-        <v>0.6000000000000001</v>
+        <v>0.7999998573213815</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -766,16 +766,16 @@
         <v>22</v>
       </c>
       <c r="B19">
-        <v>0.06230838861311393</v>
+        <v>0.9494482100330378</v>
       </c>
       <c r="C19">
-        <v>0.0452845357013687</v>
+        <v>0.9767981609654574</v>
       </c>
       <c r="D19">
-        <v>0.02297453086002567</v>
+        <v>0.9882839937274183</v>
       </c>
       <c r="E19">
-        <v>0.7000000000000002</v>
+        <v>0.8499998929910361</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -783,16 +783,16 @@
         <v>23</v>
       </c>
       <c r="B20">
-        <v>0.05612586017979098</v>
+        <v>0.9028568367635105</v>
       </c>
       <c r="C20">
-        <v>0.06307744595549693</v>
+        <v>0.9367215821998738</v>
       </c>
       <c r="D20">
-        <v>0.07235293472813044</v>
+        <v>0.944724354652655</v>
       </c>
       <c r="E20">
-        <v>0.8</v>
+        <v>0.8999999286606907</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -800,16 +800,16 @@
         <v>24</v>
       </c>
       <c r="B21">
-        <v>0.04842743529573486</v>
+        <v>0.7217200486092825</v>
       </c>
       <c r="C21">
-        <v>0.07471023587355272</v>
+        <v>0.7447144090249544</v>
       </c>
       <c r="D21">
-        <v>0.08640342437569778</v>
+        <v>0.7355765974985735</v>
       </c>
       <c r="E21">
-        <v>0.9000000000000001</v>
+        <v>0.9499999643303453</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -817,13 +817,13 @@
         <v>25</v>
       </c>
       <c r="B22">
-        <v>0.0384777</v>
+        <v>0.527168632</v>
       </c>
       <c r="C22">
-        <v>0.0493915</v>
+        <v>0.546208382</v>
       </c>
       <c r="D22">
-        <v>0.0774174</v>
+        <v>0.515793443</v>
       </c>
       <c r="E22">
         <v>1</v>

</xml_diff>

<commit_message>
Add Citation on README.md
</commit_message>
<xml_diff>
--- a/data/curve_for_gci.xlsx
+++ b/data/curve_for_gci.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t>variable</t>
   </si>
@@ -34,61 +34,298 @@
     <t>phi_-0.0000</t>
   </si>
   <si>
-    <t>phi_0.0500</t>
-  </si>
-  <si>
-    <t>phi_0.1000</t>
-  </si>
-  <si>
-    <t>phi_0.1500</t>
-  </si>
-  <si>
-    <t>phi_0.2000</t>
-  </si>
-  <si>
-    <t>phi_0.2500</t>
-  </si>
-  <si>
-    <t>phi_0.3000</t>
-  </si>
-  <si>
-    <t>phi_0.3500</t>
-  </si>
-  <si>
-    <t>phi_0.4000</t>
-  </si>
-  <si>
-    <t>phi_0.4500</t>
-  </si>
-  <si>
-    <t>phi_0.5000</t>
-  </si>
-  <si>
-    <t>phi_0.5500</t>
-  </si>
-  <si>
-    <t>phi_0.6000</t>
-  </si>
-  <si>
-    <t>phi_0.6500</t>
-  </si>
-  <si>
-    <t>phi_0.7000</t>
-  </si>
-  <si>
-    <t>phi_0.7500</t>
-  </si>
-  <si>
-    <t>phi_0.8000</t>
-  </si>
-  <si>
-    <t>phi_0.8500</t>
-  </si>
-  <si>
-    <t>phi_0.9000</t>
-  </si>
-  <si>
-    <t>phi_0.9500</t>
+    <t>phi_0.0101</t>
+  </si>
+  <si>
+    <t>phi_0.0202</t>
+  </si>
+  <si>
+    <t>phi_0.0303</t>
+  </si>
+  <si>
+    <t>phi_0.0404</t>
+  </si>
+  <si>
+    <t>phi_0.0505</t>
+  </si>
+  <si>
+    <t>phi_0.0606</t>
+  </si>
+  <si>
+    <t>phi_0.0707</t>
+  </si>
+  <si>
+    <t>phi_0.0808</t>
+  </si>
+  <si>
+    <t>phi_0.0909</t>
+  </si>
+  <si>
+    <t>phi_0.1010</t>
+  </si>
+  <si>
+    <t>phi_0.1111</t>
+  </si>
+  <si>
+    <t>phi_0.1212</t>
+  </si>
+  <si>
+    <t>phi_0.1313</t>
+  </si>
+  <si>
+    <t>phi_0.1414</t>
+  </si>
+  <si>
+    <t>phi_0.1515</t>
+  </si>
+  <si>
+    <t>phi_0.1616</t>
+  </si>
+  <si>
+    <t>phi_0.1717</t>
+  </si>
+  <si>
+    <t>phi_0.1818</t>
+  </si>
+  <si>
+    <t>phi_0.1919</t>
+  </si>
+  <si>
+    <t>phi_0.2020</t>
+  </si>
+  <si>
+    <t>phi_0.2121</t>
+  </si>
+  <si>
+    <t>phi_0.2222</t>
+  </si>
+  <si>
+    <t>phi_0.2323</t>
+  </si>
+  <si>
+    <t>phi_0.2424</t>
+  </si>
+  <si>
+    <t>phi_0.2525</t>
+  </si>
+  <si>
+    <t>phi_0.2626</t>
+  </si>
+  <si>
+    <t>phi_0.2727</t>
+  </si>
+  <si>
+    <t>phi_0.2828</t>
+  </si>
+  <si>
+    <t>phi_0.2929</t>
+  </si>
+  <si>
+    <t>phi_0.3030</t>
+  </si>
+  <si>
+    <t>phi_0.3131</t>
+  </si>
+  <si>
+    <t>phi_0.3232</t>
+  </si>
+  <si>
+    <t>phi_0.3333</t>
+  </si>
+  <si>
+    <t>phi_0.3434</t>
+  </si>
+  <si>
+    <t>phi_0.3535</t>
+  </si>
+  <si>
+    <t>phi_0.3636</t>
+  </si>
+  <si>
+    <t>phi_0.3737</t>
+  </si>
+  <si>
+    <t>phi_0.3838</t>
+  </si>
+  <si>
+    <t>phi_0.3939</t>
+  </si>
+  <si>
+    <t>phi_0.4040</t>
+  </si>
+  <si>
+    <t>phi_0.4141</t>
+  </si>
+  <si>
+    <t>phi_0.4242</t>
+  </si>
+  <si>
+    <t>phi_0.4343</t>
+  </si>
+  <si>
+    <t>phi_0.4444</t>
+  </si>
+  <si>
+    <t>phi_0.4545</t>
+  </si>
+  <si>
+    <t>phi_0.4646</t>
+  </si>
+  <si>
+    <t>phi_0.4747</t>
+  </si>
+  <si>
+    <t>phi_0.4848</t>
+  </si>
+  <si>
+    <t>phi_0.4949</t>
+  </si>
+  <si>
+    <t>phi_0.5051</t>
+  </si>
+  <si>
+    <t>phi_0.5152</t>
+  </si>
+  <si>
+    <t>phi_0.5253</t>
+  </si>
+  <si>
+    <t>phi_0.5354</t>
+  </si>
+  <si>
+    <t>phi_0.5455</t>
+  </si>
+  <si>
+    <t>phi_0.5556</t>
+  </si>
+  <si>
+    <t>phi_0.5657</t>
+  </si>
+  <si>
+    <t>phi_0.5758</t>
+  </si>
+  <si>
+    <t>phi_0.5859</t>
+  </si>
+  <si>
+    <t>phi_0.5960</t>
+  </si>
+  <si>
+    <t>phi_0.6061</t>
+  </si>
+  <si>
+    <t>phi_0.6162</t>
+  </si>
+  <si>
+    <t>phi_0.6263</t>
+  </si>
+  <si>
+    <t>phi_0.6364</t>
+  </si>
+  <si>
+    <t>phi_0.6465</t>
+  </si>
+  <si>
+    <t>phi_0.6566</t>
+  </si>
+  <si>
+    <t>phi_0.6667</t>
+  </si>
+  <si>
+    <t>phi_0.6768</t>
+  </si>
+  <si>
+    <t>phi_0.6869</t>
+  </si>
+  <si>
+    <t>phi_0.6970</t>
+  </si>
+  <si>
+    <t>phi_0.7071</t>
+  </si>
+  <si>
+    <t>phi_0.7172</t>
+  </si>
+  <si>
+    <t>phi_0.7273</t>
+  </si>
+  <si>
+    <t>phi_0.7374</t>
+  </si>
+  <si>
+    <t>phi_0.7475</t>
+  </si>
+  <si>
+    <t>phi_0.7576</t>
+  </si>
+  <si>
+    <t>phi_0.7677</t>
+  </si>
+  <si>
+    <t>phi_0.7778</t>
+  </si>
+  <si>
+    <t>phi_0.7879</t>
+  </si>
+  <si>
+    <t>phi_0.7980</t>
+  </si>
+  <si>
+    <t>phi_0.8081</t>
+  </si>
+  <si>
+    <t>phi_0.8182</t>
+  </si>
+  <si>
+    <t>phi_0.8283</t>
+  </si>
+  <si>
+    <t>phi_0.8384</t>
+  </si>
+  <si>
+    <t>phi_0.8485</t>
+  </si>
+  <si>
+    <t>phi_0.8586</t>
+  </si>
+  <si>
+    <t>phi_0.8687</t>
+  </si>
+  <si>
+    <t>phi_0.8788</t>
+  </si>
+  <si>
+    <t>phi_0.8889</t>
+  </si>
+  <si>
+    <t>phi_0.8990</t>
+  </si>
+  <si>
+    <t>phi_0.9091</t>
+  </si>
+  <si>
+    <t>phi_0.9192</t>
+  </si>
+  <si>
+    <t>phi_0.9293</t>
+  </si>
+  <si>
+    <t>phi_0.9394</t>
+  </si>
+  <si>
+    <t>phi_0.9495</t>
+  </si>
+  <si>
+    <t>phi_0.9596</t>
+  </si>
+  <si>
+    <t>phi_0.9697</t>
+  </si>
+  <si>
+    <t>phi_0.9798</t>
+  </si>
+  <si>
+    <t>phi_0.9899</t>
   </si>
   <si>
     <t>phi_1.0000</t>
@@ -449,7 +686,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -494,16 +731,16 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>0.4246112354279316</v>
+        <v>0.4434894602242762</v>
       </c>
       <c r="C3">
-        <v>0.4262847582645582</v>
+        <v>0.447079842332995</v>
       </c>
       <c r="D3">
-        <v>0.435861379980351</v>
+        <v>0.4658045210969317</v>
       </c>
       <c r="E3">
-        <v>0.04999932227656259</v>
+        <v>0.01010030391390893</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -511,16 +748,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>0.362232850563531</v>
+        <v>0.4408691188738096</v>
       </c>
       <c r="C4">
-        <v>0.3635276939148809</v>
+        <v>0.4513381690799196</v>
       </c>
       <c r="D4">
-        <v>0.3698628781433433</v>
+        <v>0.4642605994837535</v>
       </c>
       <c r="E4">
-        <v>0.09999935794621718</v>
+        <v>0.02020132122090986</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -528,16 +765,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>0.2869568017485726</v>
+        <v>0.4382529522921895</v>
       </c>
       <c r="C5">
-        <v>0.2929609431107805</v>
+        <v>0.444094699619622</v>
       </c>
       <c r="D5">
-        <v>0.2979116755464833</v>
+        <v>0.4567872380885863</v>
       </c>
       <c r="E5">
-        <v>0.1499993936158718</v>
+        <v>0.03030233852791079</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -545,16 +782,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>0.2085413773140853</v>
+        <v>0.4352935931335969</v>
       </c>
       <c r="C6">
-        <v>0.2167929287941868</v>
+        <v>0.4367096749965538</v>
       </c>
       <c r="D6">
-        <v>0.2201327974124013</v>
+        <v>0.4467287627761583</v>
       </c>
       <c r="E6">
-        <v>0.1999994292855264</v>
+        <v>0.04040335583491171</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -562,16 +799,16 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>0.1351285381754221</v>
+        <v>0.4239872813601936</v>
       </c>
       <c r="C7">
-        <v>0.1423025141596007</v>
+        <v>0.425711200122844</v>
       </c>
       <c r="D7">
-        <v>0.14372573426556</v>
+        <v>0.4352642729903109</v>
       </c>
       <c r="E7">
-        <v>0.249999464955181</v>
+        <v>0.05050437314191264</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -579,16 +816,16 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>0.07138259991756449</v>
+        <v>0.412689544438086</v>
       </c>
       <c r="C8">
-        <v>0.07674601964131285</v>
+        <v>0.4146209412718964</v>
       </c>
       <c r="D8">
-        <v>0.0771815567248072</v>
+        <v>0.4228930177145572</v>
       </c>
       <c r="E8">
-        <v>0.2999995006248355</v>
+        <v>0.06060539044891357</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -596,16 +833,16 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>0.02297510738591806</v>
+        <v>0.4014010124427904</v>
       </c>
       <c r="C9">
-        <v>0.02629345425254802</v>
+        <v>0.4019679919947338</v>
       </c>
       <c r="D9">
-        <v>0.02552679883793104</v>
+        <v>0.409881817540475</v>
       </c>
       <c r="E9">
-        <v>0.3499995362944902</v>
+        <v>0.0707064077559145</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -613,16 +850,16 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>0.04411748410674251</v>
+        <v>0.3898612380228659</v>
       </c>
       <c r="C10">
-        <v>0.04416111023660232</v>
+        <v>0.3892521979022244</v>
       </c>
       <c r="D10">
-        <v>0.03993078715810641</v>
+        <v>0.3963970033314512</v>
       </c>
       <c r="E10">
-        <v>0.3999995719641448</v>
+        <v>0.08080742506291543</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -630,16 +867,16 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>0.08988136754102584</v>
+        <v>0.3753220984501908</v>
       </c>
       <c r="C11">
-        <v>0.08991195453941069</v>
+        <v>0.3757241097919976</v>
       </c>
       <c r="D11">
-        <v>0.08629661294338958</v>
+        <v>0.382554710398131</v>
       </c>
       <c r="E11">
-        <v>0.4499996076337994</v>
+        <v>0.09090844236991635</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -647,16 +884,16 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>0.1361954070995965</v>
+        <v>0.3607908398338551</v>
       </c>
       <c r="C12">
-        <v>0.1359988540096508</v>
+        <v>0.3621551944018199</v>
       </c>
       <c r="D12">
-        <v>0.1326337387927119</v>
+        <v>0.3684414252865989</v>
       </c>
       <c r="E12">
-        <v>0.499999643303454</v>
+        <v>0.1010094596769173</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -664,16 +901,16 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>0.1840127752610901</v>
+        <v>0.3462685193914585</v>
       </c>
       <c r="C13">
-        <v>0.1821744756461599</v>
+        <v>0.3481474394702931</v>
       </c>
       <c r="D13">
-        <v>0.178864023292082</v>
+        <v>0.3541257829701615</v>
       </c>
       <c r="E13">
-        <v>0.5499996789731085</v>
+        <v>0.1111104769839182</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -681,16 +918,16 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>0.2383783516901995</v>
+        <v>0.3316154208732267</v>
       </c>
       <c r="C14">
-        <v>0.2323943639211221</v>
+        <v>0.3341147417437539</v>
       </c>
       <c r="D14">
-        <v>0.2293526279103272</v>
+        <v>0.3396617848720238</v>
       </c>
       <c r="E14">
-        <v>0.599999714642763</v>
+        <v>0.1212114942909191</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -698,16 +935,16 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>0.3127474316144384</v>
+        <v>0.3159378682965313</v>
       </c>
       <c r="C15">
-        <v>0.2995419889334269</v>
+        <v>0.3198382896080235</v>
       </c>
       <c r="D15">
-        <v>0.2986893882845401</v>
+        <v>0.3250909759442961</v>
       </c>
       <c r="E15">
-        <v>0.6499997503124176</v>
+        <v>0.1313125115979201</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -715,16 +952,16 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0.4283596859988836</v>
+        <v>0.3002681766796058</v>
       </c>
       <c r="C16">
-        <v>0.4116351294545521</v>
+        <v>0.3055012956886907</v>
       </c>
       <c r="D16">
-        <v>0.4192823897277798</v>
+        <v>0.3104407614944095</v>
       </c>
       <c r="E16">
-        <v>0.6999997859820722</v>
+        <v>0.141413528904921</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -732,16 +969,16 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>0.6075918816272678</v>
+        <v>0.2846076939305254</v>
       </c>
       <c r="C17">
-        <v>0.5950562549488467</v>
+        <v>0.2907393819215792</v>
       </c>
       <c r="D17">
-        <v>0.6147961707990083</v>
+        <v>0.2956842420896033</v>
       </c>
       <c r="E17">
-        <v>0.7499998216517269</v>
+        <v>0.151514546211922</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -749,16 +986,16 @@
         <v>21</v>
       </c>
       <c r="B18">
-        <v>0.8359285424689332</v>
+        <v>0.2689127570396474</v>
       </c>
       <c r="C18">
-        <v>0.8321582760263507</v>
+        <v>0.2758808158974274</v>
       </c>
       <c r="D18">
-        <v>0.8591015965897354</v>
+        <v>0.2806184900659927</v>
       </c>
       <c r="E18">
-        <v>0.7999998573213815</v>
+        <v>0.1616155635189229</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -766,16 +1003,16 @@
         <v>22</v>
       </c>
       <c r="B19">
-        <v>0.9494482100330378</v>
+        <v>0.2529904295923094</v>
       </c>
       <c r="C19">
-        <v>0.9767981609654574</v>
+        <v>0.2604676296090707</v>
       </c>
       <c r="D19">
-        <v>0.9882839937274183</v>
+        <v>0.2650839760891307</v>
       </c>
       <c r="E19">
-        <v>0.8499998929910361</v>
+        <v>0.1717165808259238</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -783,16 +1020,16 @@
         <v>23</v>
       </c>
       <c r="B20">
-        <v>0.9028568367635105</v>
+        <v>0.2370778928791039</v>
       </c>
       <c r="C20">
-        <v>0.9367215821998738</v>
+        <v>0.2450126175955323</v>
       </c>
       <c r="D20">
-        <v>0.944724354652655</v>
+        <v>0.2491660257294393</v>
       </c>
       <c r="E20">
-        <v>0.8999999286606907</v>
+        <v>0.1818175981329247</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -800,16 +1037,16 @@
         <v>24</v>
       </c>
       <c r="B21">
-        <v>0.7217200486092825</v>
+        <v>0.2211772930300894</v>
       </c>
       <c r="C21">
-        <v>0.7447144090249544</v>
+        <v>0.2293216897403971</v>
       </c>
       <c r="D21">
-        <v>0.7355765974985735</v>
+        <v>0.2330459901833206</v>
       </c>
       <c r="E21">
-        <v>0.9499999643303453</v>
+        <v>0.1919186154399257</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -817,15 +1054,1358 @@
         <v>25</v>
       </c>
       <c r="B22">
+        <v>0.2054414326936442</v>
+      </c>
+      <c r="C22">
+        <v>0.2136771672002225</v>
+      </c>
+      <c r="D22">
+        <v>0.2169132886782678</v>
+      </c>
+      <c r="E22">
+        <v>0.2020196327469266</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>0.1903203174217203</v>
+      </c>
+      <c r="C23">
+        <v>0.1981739967052885</v>
+      </c>
+      <c r="D23">
+        <v>0.2009231196756598</v>
+      </c>
+      <c r="E23">
+        <v>0.2121206500539275</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <v>0.1752141869631446</v>
+      </c>
+      <c r="C24">
+        <v>0.182796836115165</v>
+      </c>
+      <c r="D24">
+        <v>0.1851864234150579</v>
+      </c>
+      <c r="E24">
+        <v>0.2222216673609284</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>0.1601273111369545</v>
+      </c>
+      <c r="C25">
+        <v>0.1678208429513384</v>
+      </c>
+      <c r="D25">
+        <v>0.1697767334558681</v>
+      </c>
+      <c r="E25">
+        <v>0.2323226846679294</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26">
+        <v>0.1454009422681054</v>
+      </c>
+      <c r="C26">
+        <v>0.1530279891258793</v>
+      </c>
+      <c r="D26">
+        <v>0.1547402155930318</v>
+      </c>
+      <c r="E26">
+        <v>0.2424237019749303</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27">
+        <v>0.131764008543418</v>
+      </c>
+      <c r="C27">
+        <v>0.1387638436496985</v>
+      </c>
+      <c r="D27">
+        <v>0.1401059996759349</v>
+      </c>
+      <c r="E27">
+        <v>0.2525247192819312</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28">
+        <v>0.1181595988294775</v>
+      </c>
+      <c r="C28">
+        <v>0.124722328155697</v>
+      </c>
+      <c r="D28">
+        <v>0.1258921238947787</v>
+      </c>
+      <c r="E28">
+        <v>0.2626257365889321</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29">
+        <v>0.1046004667784932</v>
+      </c>
+      <c r="C29">
+        <v>0.1112524152511506</v>
+      </c>
+      <c r="D29">
+        <v>0.1121114394816219</v>
+      </c>
+      <c r="E29">
+        <v>0.2727267538959331</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30">
+        <v>0.09152993884549505</v>
+      </c>
+      <c r="C30">
+        <v>0.09804131859199545</v>
+      </c>
+      <c r="D30">
+        <v>0.09877602393490077</v>
+      </c>
+      <c r="E30">
+        <v>0.282827771202934</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31">
+        <v>0.07962995707883755</v>
+      </c>
+      <c r="C31">
+        <v>0.08541469872431827</v>
+      </c>
+      <c r="D31">
+        <v>0.08590285720368528</v>
+      </c>
+      <c r="E31">
+        <v>0.2929287885099349</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32">
+        <v>0.06784557817629804</v>
+      </c>
+      <c r="C32">
+        <v>0.07310830569589551</v>
+      </c>
+      <c r="D32">
+        <v>0.07352125922188357</v>
+      </c>
+      <c r="E32">
+        <v>0.3030298058169359</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33">
+        <v>0.05624952064237613</v>
+      </c>
+      <c r="C33">
+        <v>0.06143787257461295</v>
+      </c>
+      <c r="D33">
+        <v>0.0616835199165981</v>
+      </c>
+      <c r="E33">
+        <v>0.3131308231239368</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34">
+        <v>0.04535966638258656</v>
+      </c>
+      <c r="C34">
+        <v>0.05026315432411824</v>
+      </c>
+      <c r="D34">
+        <v>0.05048071735623168</v>
+      </c>
+      <c r="E34">
+        <v>0.3232318404309377</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35">
+        <v>0.03581291064405603</v>
+      </c>
+      <c r="C35">
+        <v>0.0400099762922623</v>
+      </c>
+      <c r="D35">
+        <v>0.04006627282599597</v>
+      </c>
+      <c r="E35">
+        <v>0.3333328577379386</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36">
+        <v>0.02734572071194713</v>
+      </c>
+      <c r="C36">
+        <v>0.03097345541805266</v>
+      </c>
+      <c r="D36">
+        <v>0.03072452449964267</v>
+      </c>
+      <c r="E36">
+        <v>0.3434338750449396</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37">
+        <v>0.02128785081488227</v>
+      </c>
+      <c r="C37">
+        <v>0.02436341024386641</v>
+      </c>
+      <c r="D37">
+        <v>0.02318425418072486</v>
+      </c>
+      <c r="E37">
+        <v>0.3535348923519405</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38">
+        <v>0.01994813948141927</v>
+      </c>
+      <c r="C38">
+        <v>0.0219110766795671</v>
+      </c>
+      <c r="D38">
+        <v>0.01923767439610116</v>
+      </c>
+      <c r="E38">
+        <v>0.3636359096589414</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39">
+        <v>0.02365169495842981</v>
+      </c>
+      <c r="C39">
+        <v>0.02460406640307092</v>
+      </c>
+      <c r="D39">
+        <v>0.02076444917754742</v>
+      </c>
+      <c r="E39">
+        <v>0.3737369269659424</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40">
+        <v>0.03047331344887078</v>
+      </c>
+      <c r="C40">
+        <v>0.03091965968734514</v>
+      </c>
+      <c r="D40">
+        <v>0.02667030803678193</v>
+      </c>
+      <c r="E40">
+        <v>0.3838379442729433</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41">
+        <v>0.03880191280271777</v>
+      </c>
+      <c r="C41">
+        <v>0.03893413425601047</v>
+      </c>
+      <c r="D41">
+        <v>0.03467153868359383</v>
+      </c>
+      <c r="E41">
+        <v>0.3939389615799442</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42">
+        <v>0.04771153922678272</v>
+      </c>
+      <c r="C42">
+        <v>0.04773777628420785</v>
+      </c>
+      <c r="D42">
+        <v>0.04354393973838925</v>
+      </c>
+      <c r="E42">
+        <v>0.4040399788869452</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43">
+        <v>0.05676454891860182</v>
+      </c>
+      <c r="C43">
+        <v>0.05683046143469156</v>
+      </c>
+      <c r="D43">
+        <v>0.05278633725672637</v>
+      </c>
+      <c r="E43">
+        <v>0.4141409961939461</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44">
+        <v>0.06602154241454641</v>
+      </c>
+      <c r="C44">
+        <v>0.06610122568220252</v>
+      </c>
+      <c r="D44">
+        <v>0.06218471847659031</v>
+      </c>
+      <c r="E44">
+        <v>0.424242013500947</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45">
+        <v>0.07540741718118747</v>
+      </c>
+      <c r="C45">
+        <v>0.07541308603866449</v>
+      </c>
+      <c r="D45">
+        <v>0.07163922008982983</v>
+      </c>
+      <c r="E45">
+        <v>0.4343430308079479</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46">
+        <v>0.0847720172882023</v>
+      </c>
+      <c r="C46">
+        <v>0.08476896329088453</v>
+      </c>
+      <c r="D46">
+        <v>0.08110009778158529</v>
+      </c>
+      <c r="E46">
+        <v>0.4444440481149489</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47">
+        <v>0.0940578146619882</v>
+      </c>
+      <c r="C47">
+        <v>0.0941178448386031</v>
+      </c>
+      <c r="D47">
+        <v>0.0905424093397911</v>
+      </c>
+      <c r="E47">
+        <v>0.4545450654219498</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48">
+        <v>0.1033850827638027</v>
+      </c>
+      <c r="C48">
+        <v>0.1034632615130007</v>
+      </c>
+      <c r="D48">
+        <v>0.09995441929384431</v>
+      </c>
+      <c r="E48">
+        <v>0.4646460827289507</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49">
+        <v>0.112743515625199</v>
+      </c>
+      <c r="C49">
+        <v>0.1127817067444704</v>
+      </c>
+      <c r="D49">
+        <v>0.1093316415081418</v>
+      </c>
+      <c r="E49">
+        <v>0.4747471000359517</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50">
+        <v>0.1221155392360977</v>
+      </c>
+      <c r="C50">
+        <v>0.1220846029376494</v>
+      </c>
+      <c r="D50">
+        <v>0.1186742045061248</v>
+      </c>
+      <c r="E50">
+        <v>0.4848481173429526</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51">
+        <v>0.1314958400266185</v>
+      </c>
+      <c r="C51">
+        <v>0.1313618472251668</v>
+      </c>
+      <c r="D51">
+        <v>0.1279864816179459</v>
+      </c>
+      <c r="E51">
+        <v>0.4949491346499535</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52">
+        <v>0.1408920324199714</v>
+      </c>
+      <c r="C52">
+        <v>0.1406333166856801</v>
+      </c>
+      <c r="D52">
+        <v>0.1372770389861071</v>
+      </c>
+      <c r="E52">
+        <v>0.5050501519569544</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53">
+        <v>0.1503011755623748</v>
+      </c>
+      <c r="C53">
+        <v>0.1498958313919059</v>
+      </c>
+      <c r="D53">
+        <v>0.1465595205207955</v>
+      </c>
+      <c r="E53">
+        <v>0.5151511692639553</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>57</v>
+      </c>
+      <c r="B54">
+        <v>0.1599334367401333</v>
+      </c>
+      <c r="C54">
+        <v>0.1591872992189874</v>
+      </c>
+      <c r="D54">
+        <v>0.1558537303850651</v>
+      </c>
+      <c r="E54">
+        <v>0.5252521865709562</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55">
+        <v>0.1697724328774921</v>
+      </c>
+      <c r="C55">
+        <v>0.1685048137515526</v>
+      </c>
+      <c r="D55">
+        <v>0.1651869217409564</v>
+      </c>
+      <c r="E55">
+        <v>0.5353532038779572</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56">
+        <v>0.1796207847510481</v>
+      </c>
+      <c r="C56">
+        <v>0.1779197093068328</v>
+      </c>
+      <c r="D56">
+        <v>0.174594574530873</v>
+      </c>
+      <c r="E56">
+        <v>0.5454542211849581</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57">
+        <v>0.1894770260387485</v>
+      </c>
+      <c r="C57">
+        <v>0.1874181409423205</v>
+      </c>
+      <c r="D57">
+        <v>0.1841224509543305</v>
+      </c>
+      <c r="E57">
+        <v>0.555555238491959</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>61</v>
+      </c>
+      <c r="B58">
+        <v>0.2000439234216977</v>
+      </c>
+      <c r="C58">
+        <v>0.197133279628934</v>
+      </c>
+      <c r="D58">
+        <v>0.1938293051843928</v>
+      </c>
+      <c r="E58">
+        <v>0.56565625579896</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59">
+        <v>0.2111722453440824</v>
+      </c>
+      <c r="C59">
+        <v>0.2070200970229265</v>
+      </c>
+      <c r="D59">
+        <v>0.203789927309202</v>
+      </c>
+      <c r="E59">
+        <v>0.5757572731059609</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60">
+        <v>0.2223082186869965</v>
+      </c>
+      <c r="C60">
+        <v>0.2173222542523758</v>
+      </c>
+      <c r="D60">
+        <v>0.2140991495872528</v>
+      </c>
+      <c r="E60">
+        <v>0.5858582904129618</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B61">
+        <v>0.2334507777709945</v>
+      </c>
+      <c r="C61">
+        <v>0.227927428184346</v>
+      </c>
+      <c r="D61">
+        <v>0.2248772661854471</v>
+      </c>
+      <c r="E61">
+        <v>0.5959593077199627</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>65</v>
+      </c>
+      <c r="B62">
+        <v>0.2463178294248691</v>
+      </c>
+      <c r="C62">
+        <v>0.2392704496705751</v>
+      </c>
+      <c r="D62">
+        <v>0.2362765555237774</v>
+      </c>
+      <c r="E62">
+        <v>0.6060603250269637</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63">
+        <v>0.2603391244423253</v>
+      </c>
+      <c r="C63">
+        <v>0.2511084613237328</v>
+      </c>
+      <c r="D63">
+        <v>0.248486737890765</v>
+      </c>
+      <c r="E63">
+        <v>0.6161613423339646</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64">
+        <v>0.2743680193071437</v>
+      </c>
+      <c r="C64">
+        <v>0.2641888547777461</v>
+      </c>
+      <c r="D64">
+        <v>0.2617420002777893</v>
+      </c>
+      <c r="E64">
+        <v>0.6262623596409655</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65">
+        <v>0.2884034999194866</v>
+      </c>
+      <c r="C65">
+        <v>0.2780347579721404</v>
+      </c>
+      <c r="D65">
+        <v>0.2763249445850038</v>
+      </c>
+      <c r="E65">
+        <v>0.6363633769479664</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>69</v>
+      </c>
+      <c r="B66">
+        <v>0.305999568087381</v>
+      </c>
+      <c r="C66">
+        <v>0.2938354828591382</v>
+      </c>
+      <c r="D66">
+        <v>0.2925567345904456</v>
+      </c>
+      <c r="E66">
+        <v>0.6464643942549674</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67">
+        <v>0.3256033005285711</v>
+      </c>
+      <c r="C67">
+        <v>0.3107406869723364</v>
+      </c>
+      <c r="D67">
+        <v>0.3107736282020962</v>
+      </c>
+      <c r="E67">
+        <v>0.6565654115619683</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>71</v>
+      </c>
+      <c r="B68">
+        <v>0.3452140462382771</v>
+      </c>
+      <c r="C68">
+        <v>0.3304436128884421</v>
+      </c>
+      <c r="D68">
+        <v>0.3313184747754264</v>
+      </c>
+      <c r="E68">
+        <v>0.6666664288689692</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69">
+        <v>0.3648306793921363</v>
+      </c>
+      <c r="C69">
+        <v>0.351592880952407</v>
+      </c>
+      <c r="D69">
+        <v>0.3545229119314197</v>
+      </c>
+      <c r="E69">
+        <v>0.6767674461759702</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>73</v>
+      </c>
+      <c r="B70">
+        <v>0.3907212233240239</v>
+      </c>
+      <c r="C70">
+        <v>0.3763470332166319</v>
+      </c>
+      <c r="D70">
+        <v>0.3806501499777115</v>
+      </c>
+      <c r="E70">
+        <v>0.686868463482971</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71">
+        <v>0.4195672524123725</v>
+      </c>
+      <c r="C71">
+        <v>0.4028020687546741</v>
+      </c>
+      <c r="D71">
+        <v>0.4098880081210955</v>
+      </c>
+      <c r="E71">
+        <v>0.696969480789972</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>75</v>
+      </c>
+      <c r="B72">
+        <v>0.4484175178892629</v>
+      </c>
+      <c r="C72">
+        <v>0.4334439407652479</v>
+      </c>
+      <c r="D72">
+        <v>0.4423320880594328</v>
+      </c>
+      <c r="E72">
+        <v>0.707070498096973</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>76</v>
+      </c>
+      <c r="B73">
+        <v>0.4772712356387407</v>
+      </c>
+      <c r="C73">
+        <v>0.465883157629718</v>
+      </c>
+      <c r="D73">
+        <v>0.4779994623586016</v>
+      </c>
+      <c r="E73">
+        <v>0.7171715154039738</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>77</v>
+      </c>
+      <c r="B74">
+        <v>0.515031845745659</v>
+      </c>
+      <c r="C74">
+        <v>0.5027396152738379</v>
+      </c>
+      <c r="D74">
+        <v>0.5168180754122988</v>
+      </c>
+      <c r="E74">
+        <v>0.7272725327109748</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>78</v>
+      </c>
+      <c r="B75">
+        <v>0.5562563208890199</v>
+      </c>
+      <c r="C75">
+        <v>0.5413152782656984</v>
+      </c>
+      <c r="D75">
+        <v>0.5586400433903053</v>
+      </c>
+      <c r="E75">
+        <v>0.7373735500179758</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>79</v>
+      </c>
+      <c r="B76">
+        <v>0.5974813746469979</v>
+      </c>
+      <c r="C76">
+        <v>0.5841354409662738</v>
+      </c>
+      <c r="D76">
+        <v>0.6032445272861029</v>
+      </c>
+      <c r="E76">
+        <v>0.7474745673249766</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>80</v>
+      </c>
+      <c r="B77">
+        <v>0.6387068176557695</v>
+      </c>
+      <c r="C77">
+        <v>0.6284473257901623</v>
+      </c>
+      <c r="D77">
+        <v>0.6503126502942053</v>
+      </c>
+      <c r="E77">
+        <v>0.7575755846319776</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>81</v>
+      </c>
+      <c r="B78">
+        <v>0.6849204630123205</v>
+      </c>
+      <c r="C78">
+        <v>0.676030196916687</v>
+      </c>
+      <c r="D78">
+        <v>0.6993745441695023</v>
+      </c>
+      <c r="E78">
+        <v>0.7676766019389786</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>82</v>
+      </c>
+      <c r="B79">
+        <v>0.7327100752161827</v>
+      </c>
+      <c r="C79">
+        <v>0.7246460532027197</v>
+      </c>
+      <c r="D79">
+        <v>0.7497307404339792</v>
+      </c>
+      <c r="E79">
+        <v>0.7777776192459794</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>83</v>
+      </c>
+      <c r="B80">
+        <v>0.7805006058862487</v>
+      </c>
+      <c r="C80">
+        <v>0.7737834029619655</v>
+      </c>
+      <c r="D80">
+        <v>0.8003254121371319</v>
+      </c>
+      <c r="E80">
+        <v>0.7878786365529804</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>84</v>
+      </c>
+      <c r="B81">
+        <v>0.8282918391729206</v>
+      </c>
+      <c r="C81">
+        <v>0.8230680633040841</v>
+      </c>
+      <c r="D81">
+        <v>0.8495925566720504</v>
+      </c>
+      <c r="E81">
+        <v>0.7979796538599813</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>85</v>
+      </c>
+      <c r="B82">
+        <v>0.8606342506839447</v>
+      </c>
+      <c r="C82">
+        <v>0.8671149749007587</v>
+      </c>
+      <c r="D82">
+        <v>0.8952812602238535</v>
+      </c>
+      <c r="E82">
+        <v>0.8080806711669822</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>86</v>
+      </c>
+      <c r="B83">
+        <v>0.8891139332053699</v>
+      </c>
+      <c r="C83">
+        <v>0.909852877937472</v>
+      </c>
+      <c r="D83">
+        <v>0.9344714967901943</v>
+      </c>
+      <c r="E83">
+        <v>0.8181816884739832</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>87</v>
+      </c>
+      <c r="B84">
+        <v>0.9175938802109318</v>
+      </c>
+      <c r="C84">
+        <v>0.939467637140104</v>
+      </c>
+      <c r="D84">
+        <v>0.9640116126662883</v>
+      </c>
+      <c r="E84">
+        <v>0.8282827057809841</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>88</v>
+      </c>
+      <c r="B85">
+        <v>0.9460737902259231</v>
+      </c>
+      <c r="C85">
+        <v>0.9662012729890312</v>
+      </c>
+      <c r="D85">
+        <v>0.9818169427476325</v>
+      </c>
+      <c r="E85">
+        <v>0.838383723087985</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>89</v>
+      </c>
+      <c r="B86">
+        <v>0.9496942074242903</v>
+      </c>
+      <c r="C86">
+        <v>0.9756974289974518</v>
+      </c>
+      <c r="D86">
+        <v>0.9880286555407227</v>
+      </c>
+      <c r="E86">
+        <v>0.8484847403949859</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>90</v>
+      </c>
+      <c r="B87">
+        <v>0.9485791266901519</v>
+      </c>
+      <c r="C87">
+        <v>0.9819098763445815</v>
+      </c>
+      <c r="D87">
+        <v>0.9878282467239953</v>
+      </c>
+      <c r="E87">
+        <v>0.8585857577019869</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
+        <v>91</v>
+      </c>
+      <c r="B88">
+        <v>0.9474640535879684</v>
+      </c>
+      <c r="C88">
+        <v>0.9782413673069669</v>
+      </c>
+      <c r="D88">
+        <v>0.9846458268503825</v>
+      </c>
+      <c r="E88">
+        <v>0.8686867750089878</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
+        <v>92</v>
+      </c>
+      <c r="B89">
+        <v>0.9463488702264242</v>
+      </c>
+      <c r="C89">
+        <v>0.97296406912957</v>
+      </c>
+      <c r="D89">
+        <v>0.9784204054297596</v>
+      </c>
+      <c r="E89">
+        <v>0.8787877923159887</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" t="s">
+        <v>93</v>
+      </c>
+      <c r="B90">
+        <v>0.9269729689044998</v>
+      </c>
+      <c r="C90">
+        <v>0.9568245454714693</v>
+      </c>
+      <c r="D90">
+        <v>0.9667149269368707</v>
+      </c>
+      <c r="E90">
+        <v>0.8888888096229897</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>94</v>
+      </c>
+      <c r="B91">
+        <v>0.9051070148261651</v>
+      </c>
+      <c r="C91">
+        <v>0.9392036686506973</v>
+      </c>
+      <c r="D91">
+        <v>0.9471607691399725</v>
+      </c>
+      <c r="E91">
+        <v>0.8989898269299906</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" t="s">
+        <v>95</v>
+      </c>
+      <c r="B92">
+        <v>0.8832415427614233</v>
+      </c>
+      <c r="C92">
+        <v>0.9093140127293255</v>
+      </c>
+      <c r="D92">
+        <v>0.918836266993361</v>
+      </c>
+      <c r="E92">
+        <v>0.9090908442369915</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" t="s">
+        <v>96</v>
+      </c>
+      <c r="B93">
+        <v>0.8613764441790839</v>
+      </c>
+      <c r="C93">
+        <v>0.8780610871372494</v>
+      </c>
+      <c r="D93">
+        <v>0.882111510148877</v>
+      </c>
+      <c r="E93">
+        <v>0.9191918615439925</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" t="s">
+        <v>97</v>
+      </c>
+      <c r="B94">
+        <v>0.8169260807936181</v>
+      </c>
+      <c r="C94">
+        <v>0.8365025234144604</v>
+      </c>
+      <c r="D94">
+        <v>0.8379864906011336</v>
+      </c>
+      <c r="E94">
+        <v>0.9292928788509934</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" t="s">
+        <v>98</v>
+      </c>
+      <c r="B95">
+        <v>0.7705148831007249</v>
+      </c>
+      <c r="C95">
+        <v>0.7940480515038595</v>
+      </c>
+      <c r="D95">
+        <v>0.7887932341509482</v>
+      </c>
+      <c r="E95">
+        <v>0.9393938961579943</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" t="s">
+        <v>99</v>
+      </c>
+      <c r="B96">
+        <v>0.7241076100090309</v>
+      </c>
+      <c r="C96">
+        <v>0.747130141031292</v>
+      </c>
+      <c r="D96">
+        <v>0.7380918089147667</v>
+      </c>
+      <c r="E96">
+        <v>0.9494949134649953</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" t="s">
+        <v>100</v>
+      </c>
+      <c r="B97">
+        <v>0.6777051198507827</v>
+      </c>
+      <c r="C97">
+        <v>0.699930257696616</v>
+      </c>
+      <c r="D97">
+        <v>0.6889331384693356</v>
+      </c>
+      <c r="E97">
+        <v>0.9595959307719961</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>101</v>
+      </c>
+      <c r="B98">
+        <v>0.639782277093465</v>
+      </c>
+      <c r="C98">
+        <v>0.6564974983904981</v>
+      </c>
+      <c r="D98">
+        <v>0.6431663236006122</v>
+      </c>
+      <c r="E98">
+        <v>0.9696969480789971</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>102</v>
+      </c>
+      <c r="B99">
+        <v>0.6022264120895905</v>
+      </c>
+      <c r="C99">
+        <v>0.6132418263988015</v>
+      </c>
+      <c r="D99">
+        <v>0.6011240824329355</v>
+      </c>
+      <c r="E99">
+        <v>0.9797979653859981</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>103</v>
+      </c>
+      <c r="B100">
+        <v>0.5646873020306484</v>
+      </c>
+      <c r="C100">
+        <v>0.5796145717540642</v>
+      </c>
+      <c r="D100">
+        <v>0.5608328469615189</v>
+      </c>
+      <c r="E100">
+        <v>0.9898989826929989</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" t="s">
+        <v>104</v>
+      </c>
+      <c r="B101">
         <v>0.527168632</v>
       </c>
-      <c r="C22">
+      <c r="C101">
         <v>0.546208382</v>
       </c>
-      <c r="D22">
+      <c r="D101">
         <v>0.515793443</v>
       </c>
-      <c r="E22">
+      <c r="E101">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove Duplicates from Curves
</commit_message>
<xml_diff>
--- a/data/curve_for_gci.xlsx
+++ b/data/curve_for_gci.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>variable</t>
   </si>
@@ -34,61 +34,151 @@
     <t>phi_0.0000</t>
   </si>
   <si>
-    <t>phi_12.0000</t>
+    <t>phi_4.8000</t>
+  </si>
+  <si>
+    <t>phi_9.6000</t>
+  </si>
+  <si>
+    <t>phi_14.4000</t>
+  </si>
+  <si>
+    <t>phi_19.2000</t>
   </si>
   <si>
     <t>phi_24.0000</t>
   </si>
   <si>
-    <t>phi_36.0000</t>
+    <t>phi_28.8000</t>
+  </si>
+  <si>
+    <t>phi_33.6000</t>
+  </si>
+  <si>
+    <t>phi_38.4000</t>
+  </si>
+  <si>
+    <t>phi_43.2000</t>
   </si>
   <si>
     <t>phi_48.0000</t>
   </si>
   <si>
-    <t>phi_60.0000</t>
+    <t>phi_52.8000</t>
+  </si>
+  <si>
+    <t>phi_57.6000</t>
+  </si>
+  <si>
+    <t>phi_62.4000</t>
+  </si>
+  <si>
+    <t>phi_67.2000</t>
   </si>
   <si>
     <t>phi_72.0000</t>
   </si>
   <si>
-    <t>phi_84.0000</t>
+    <t>phi_76.8000</t>
+  </si>
+  <si>
+    <t>phi_81.6000</t>
+  </si>
+  <si>
+    <t>phi_86.4000</t>
+  </si>
+  <si>
+    <t>phi_91.2000</t>
   </si>
   <si>
     <t>phi_96.0000</t>
   </si>
   <si>
-    <t>phi_108.0000</t>
+    <t>phi_100.8000</t>
+  </si>
+  <si>
+    <t>phi_105.6000</t>
+  </si>
+  <si>
+    <t>phi_110.4000</t>
+  </si>
+  <si>
+    <t>phi_115.2000</t>
   </si>
   <si>
     <t>phi_120.0000</t>
   </si>
   <si>
-    <t>phi_132.0000</t>
+    <t>phi_124.8000</t>
+  </si>
+  <si>
+    <t>phi_129.6000</t>
+  </si>
+  <si>
+    <t>phi_134.4000</t>
+  </si>
+  <si>
+    <t>phi_139.2000</t>
   </si>
   <si>
     <t>phi_144.0000</t>
   </si>
   <si>
-    <t>phi_156.0000</t>
+    <t>phi_148.8000</t>
+  </si>
+  <si>
+    <t>phi_153.6000</t>
+  </si>
+  <si>
+    <t>phi_158.4000</t>
+  </si>
+  <si>
+    <t>phi_163.2000</t>
   </si>
   <si>
     <t>phi_168.0000</t>
   </si>
   <si>
-    <t>phi_180.0000</t>
+    <t>phi_172.8000</t>
+  </si>
+  <si>
+    <t>phi_177.6000</t>
+  </si>
+  <si>
+    <t>phi_182.4000</t>
+  </si>
+  <si>
+    <t>phi_187.2000</t>
   </si>
   <si>
     <t>phi_192.0000</t>
   </si>
   <si>
-    <t>phi_204.0000</t>
+    <t>phi_196.8000</t>
+  </si>
+  <si>
+    <t>phi_201.6000</t>
+  </si>
+  <si>
+    <t>phi_206.4000</t>
+  </si>
+  <si>
+    <t>phi_211.2000</t>
   </si>
   <si>
     <t>phi_216.0000</t>
   </si>
   <si>
-    <t>phi_228.0000</t>
+    <t>phi_220.8000</t>
+  </si>
+  <si>
+    <t>phi_225.6000</t>
+  </si>
+  <si>
+    <t>phi_230.4000</t>
+  </si>
+  <si>
+    <t>phi_235.2000</t>
   </si>
   <si>
     <t>phi_240.0000</t>
@@ -449,7 +539,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -503,7 +593,7 @@
         <v>2.5</v>
       </c>
       <c r="E3">
-        <v>12</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -511,16 +601,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>2.499999999999999</v>
+        <v>2.500000000000001</v>
       </c>
       <c r="C4">
-        <v>2.499999999999992</v>
+        <v>2.5</v>
       </c>
       <c r="D4">
         <v>2.5</v>
       </c>
       <c r="E4">
-        <v>24</v>
+        <v>9.6</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -528,16 +618,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>2.500000011373591</v>
+        <v>2.5</v>
       </c>
       <c r="C5">
-        <v>2.499999998254081</v>
+        <v>2.5</v>
       </c>
       <c r="D5">
-        <v>2.500000000027512</v>
+        <v>2.5</v>
       </c>
       <c r="E5">
-        <v>36</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -545,16 +635,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>2.500089309581067</v>
+        <v>2.5</v>
       </c>
       <c r="C6">
-        <v>2.489592129769505</v>
+        <v>2.500000000000001</v>
       </c>
       <c r="D6">
-        <v>2.499241292073199</v>
+        <v>2.5</v>
       </c>
       <c r="E6">
-        <v>48</v>
+        <v>19.2</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -562,16 +652,16 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>2.489999982692347</v>
+        <v>2.499999999999999</v>
       </c>
       <c r="C7">
-        <v>2.490000030471755</v>
+        <v>2.499999999999992</v>
       </c>
       <c r="D7">
-        <v>2.49000000002565</v>
+        <v>2.5</v>
       </c>
       <c r="E7">
-        <v>60</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -579,16 +669,16 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>2.490000124105086</v>
+        <v>2.5</v>
       </c>
       <c r="C8">
-        <v>2.490000001250805</v>
+        <v>2.499999999997784</v>
       </c>
       <c r="D8">
-        <v>2.490000000004322</v>
+        <v>2.5</v>
       </c>
       <c r="E8">
-        <v>72</v>
+        <v>28.8</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -596,16 +686,16 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>2.481564062242776</v>
+        <v>2.499999999957664</v>
       </c>
       <c r="C9">
-        <v>2.480000019885803</v>
+        <v>2.499999999943373</v>
       </c>
       <c r="D9">
-        <v>2.487625126096197</v>
+        <v>2.499999999999766</v>
       </c>
       <c r="E9">
-        <v>84</v>
+        <v>33.6</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -613,16 +703,16 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>2.480000023074927</v>
+        <v>2.50000001864291</v>
       </c>
       <c r="C10">
-        <v>2.480000017856514</v>
+        <v>2.500000621310545</v>
       </c>
       <c r="D10">
-        <v>2.479999999968659</v>
+        <v>2.499999999967873</v>
       </c>
       <c r="E10">
-        <v>96</v>
+        <v>38.4</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -630,16 +720,16 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>2.47502610345906</v>
+        <v>2.499999528267525</v>
       </c>
       <c r="C11">
-        <v>2.47</v>
+        <v>2.499990524110827</v>
       </c>
       <c r="D11">
-        <v>2.48</v>
+        <v>2.499999807560376</v>
       </c>
       <c r="E11">
-        <v>108</v>
+        <v>43.2</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -647,16 +737,16 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>2.469997636749464</v>
+        <v>2.500089309581067</v>
       </c>
       <c r="C12">
-        <v>2.470000000000001</v>
+        <v>2.489592129769505</v>
       </c>
       <c r="D12">
-        <v>2.47</v>
+        <v>2.499241292073199</v>
       </c>
       <c r="E12">
-        <v>120</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -664,16 +754,16 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>2.47</v>
+        <v>2.489984388705178</v>
       </c>
       <c r="C13">
-        <v>2.46</v>
+        <v>2.49</v>
       </c>
       <c r="D13">
-        <v>2.47</v>
+        <v>2.490005710692944</v>
       </c>
       <c r="E13">
-        <v>132</v>
+        <v>52.8</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -681,16 +771,16 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>2.459998659875041</v>
+        <v>2.489999935043771</v>
       </c>
       <c r="C14">
-        <v>2.450000000000001</v>
+        <v>2.489999606291078</v>
       </c>
       <c r="D14">
-        <v>2.46</v>
+        <v>2.489999999636112</v>
       </c>
       <c r="E14">
-        <v>144</v>
+        <v>57.59999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -698,16 +788,16 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>2.449858316605563</v>
+        <v>2.490000002089177</v>
       </c>
       <c r="C15">
-        <v>2.449919081809071</v>
+        <v>2.49</v>
       </c>
       <c r="D15">
-        <v>2.45</v>
+        <v>2.48999999999997</v>
       </c>
       <c r="E15">
-        <v>156</v>
+        <v>62.4</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -715,16 +805,16 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>2.44</v>
+        <v>2.489999997593245</v>
       </c>
       <c r="C16">
-        <v>2.44057325361891</v>
+        <v>2.49000000000109</v>
       </c>
       <c r="D16">
-        <v>2.45</v>
+        <v>2.490000000000001</v>
       </c>
       <c r="E16">
-        <v>168</v>
+        <v>67.2</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -732,16 +822,16 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>2.440154498405617</v>
+        <v>2.490000124105086</v>
       </c>
       <c r="C17">
-        <v>2.440002082757702</v>
+        <v>2.490000001250805</v>
       </c>
       <c r="D17">
-        <v>2.44</v>
+        <v>2.490000000004322</v>
       </c>
       <c r="E17">
-        <v>180</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -749,16 +839,16 @@
         <v>21</v>
       </c>
       <c r="B18">
-        <v>2.429891751224342</v>
+        <v>2.489995072640924</v>
       </c>
       <c r="C18">
-        <v>2.429342857480136</v>
+        <v>2.489998289627142</v>
       </c>
       <c r="D18">
-        <v>2.44</v>
+        <v>2.489999982636934</v>
       </c>
       <c r="E18">
-        <v>192</v>
+        <v>76.8</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -766,16 +856,16 @@
         <v>22</v>
       </c>
       <c r="B19">
-        <v>2.420015399734612</v>
+        <v>2.489589667744992</v>
       </c>
       <c r="C19">
-        <v>2.43</v>
+        <v>2.482785794185848</v>
       </c>
       <c r="D19">
-        <v>2.43</v>
+        <v>2.489903834948081</v>
       </c>
       <c r="E19">
-        <v>204</v>
+        <v>81.59999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -783,16 +873,16 @@
         <v>23</v>
       </c>
       <c r="B20">
-        <v>2.41</v>
+        <v>2.479915851693828</v>
       </c>
       <c r="C20">
-        <v>2.419999280486741</v>
+        <v>2.479999978924453</v>
       </c>
       <c r="D20">
-        <v>2.43</v>
+        <v>2.479966340731228</v>
       </c>
       <c r="E20">
-        <v>216</v>
+        <v>86.39999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -800,16 +890,16 @@
         <v>24</v>
       </c>
       <c r="B21">
-        <v>2.400375561335369</v>
+        <v>2.479998647733882</v>
       </c>
       <c r="C21">
-        <v>2.41</v>
+        <v>2.48</v>
       </c>
       <c r="D21">
-        <v>2.42</v>
+        <v>2.48000001382325</v>
       </c>
       <c r="E21">
-        <v>228</v>
+        <v>91.2</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -817,15 +907,525 @@
         <v>25</v>
       </c>
       <c r="B22">
+        <v>2.480000023074927</v>
+      </c>
+      <c r="C22">
+        <v>2.480000017856514</v>
+      </c>
+      <c r="D22">
+        <v>2.479999999968659</v>
+      </c>
+      <c r="E22">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>2.479997627025508</v>
+      </c>
+      <c r="C23">
+        <v>2.480069810298436</v>
+      </c>
+      <c r="D23">
+        <v>2.480000021515848</v>
+      </c>
+      <c r="E23">
+        <v>100.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <v>2.480128384614189</v>
+      </c>
+      <c r="C24">
+        <v>2.474587280817985</v>
+      </c>
+      <c r="D24">
+        <v>2.479971231542768</v>
+      </c>
+      <c r="E24">
+        <v>105.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>2.469852820895288</v>
+      </c>
+      <c r="C25">
+        <v>2.470073905180516</v>
+      </c>
+      <c r="D25">
+        <v>2.476175666480674</v>
+      </c>
+      <c r="E25">
+        <v>110.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26">
+        <v>2.469995007751593</v>
+      </c>
+      <c r="C26">
+        <v>2.470002575332223</v>
+      </c>
+      <c r="D26">
+        <v>2.470039152626418</v>
+      </c>
+      <c r="E26">
+        <v>115.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27">
+        <v>2.469997636749464</v>
+      </c>
+      <c r="C27">
+        <v>2.470000000000001</v>
+      </c>
+      <c r="D27">
+        <v>2.47</v>
+      </c>
+      <c r="E27">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28">
+        <v>2.470117890106914</v>
+      </c>
+      <c r="C28">
+        <v>2.45984406491221</v>
+      </c>
+      <c r="D28">
+        <v>2.46999769032744</v>
+      </c>
+      <c r="E28">
+        <v>124.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29">
+        <v>2.474886292254106</v>
+      </c>
+      <c r="C29">
+        <v>2.460027896587066</v>
+      </c>
+      <c r="D29">
+        <v>2.470146529943916</v>
+      </c>
+      <c r="E29">
+        <v>129.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30">
+        <v>2.460532671350595</v>
+      </c>
+      <c r="C30">
+        <v>2.460000166266445</v>
+      </c>
+      <c r="D30">
+        <v>2.458505065318633</v>
+      </c>
+      <c r="E30">
+        <v>134.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31">
+        <v>2.460022462619984</v>
+      </c>
+      <c r="C31">
+        <v>2.460010995631992</v>
+      </c>
+      <c r="D31">
+        <v>2.459990599412635</v>
+      </c>
+      <c r="E31">
+        <v>139.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32">
+        <v>2.459998659875041</v>
+      </c>
+      <c r="C32">
+        <v>2.450000000000001</v>
+      </c>
+      <c r="D32">
+        <v>2.46</v>
+      </c>
+      <c r="E32">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33">
+        <v>2.46086607858413</v>
+      </c>
+      <c r="C33">
+        <v>2.450002718683725</v>
+      </c>
+      <c r="D33">
+        <v>2.459994274753182</v>
+      </c>
+      <c r="E33">
+        <v>148.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34">
+        <v>2.449725024491662</v>
+      </c>
+      <c r="C34">
+        <v>2.450004064495556</v>
+      </c>
+      <c r="D34">
+        <v>2.45744947661752</v>
+      </c>
+      <c r="E34">
+        <v>153.6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35">
+        <v>2.44995555023679</v>
+      </c>
+      <c r="C35">
+        <v>2.450296674865006</v>
+      </c>
+      <c r="D35">
+        <v>2.44996066687972</v>
+      </c>
+      <c r="E35">
+        <v>158.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36">
+        <v>2.451041857992208</v>
+      </c>
+      <c r="C36">
+        <v>2.453603109105049</v>
+      </c>
+      <c r="D36">
+        <v>2.449999812494139</v>
+      </c>
+      <c r="E36">
+        <v>163.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37">
+        <v>2.44</v>
+      </c>
+      <c r="C37">
+        <v>2.44057325361891</v>
+      </c>
+      <c r="D37">
+        <v>2.45</v>
+      </c>
+      <c r="E37">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38">
+        <v>2.439958616148652</v>
+      </c>
+      <c r="C38">
+        <v>2.439998405946219</v>
+      </c>
+      <c r="D38">
+        <v>2.45005979552858</v>
+      </c>
+      <c r="E38">
+        <v>172.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39">
+        <v>2.440011103623555</v>
+      </c>
+      <c r="C39">
+        <v>2.440000035188972</v>
+      </c>
+      <c r="D39">
+        <v>2.441484957578088</v>
+      </c>
+      <c r="E39">
+        <v>177.6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40">
+        <v>2.439353156586585</v>
+      </c>
+      <c r="C40">
+        <v>2.439997093402673</v>
+      </c>
+      <c r="D40">
+        <v>2.439997969616683</v>
+      </c>
+      <c r="E40">
+        <v>182.4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41">
+        <v>2.427991709732975</v>
+      </c>
+      <c r="C41">
+        <v>2.439714830212853</v>
+      </c>
+      <c r="D41">
+        <v>2.440000071099023</v>
+      </c>
+      <c r="E41">
+        <v>187.2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42">
+        <v>2.429891751224342</v>
+      </c>
+      <c r="C42">
+        <v>2.429342857480136</v>
+      </c>
+      <c r="D42">
+        <v>2.44</v>
+      </c>
+      <c r="E42">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43">
+        <v>2.428251148349782</v>
+      </c>
+      <c r="C43">
+        <v>2.430001403802158</v>
+      </c>
+      <c r="D43">
+        <v>2.440061791899504</v>
+      </c>
+      <c r="E43">
+        <v>196.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44">
+        <v>2.420073546690566</v>
+      </c>
+      <c r="C44">
+        <v>2.43000465076093</v>
+      </c>
+      <c r="D44">
+        <v>2.430706736401744</v>
+      </c>
+      <c r="E44">
+        <v>201.6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45">
+        <v>2.420191976584769</v>
+      </c>
+      <c r="C45">
+        <v>2.432262007177107</v>
+      </c>
+      <c r="D45">
+        <v>2.429993089233683</v>
+      </c>
+      <c r="E45">
+        <v>206.4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46">
+        <v>2.412129410318576</v>
+      </c>
+      <c r="C46">
+        <v>2.418285522693018</v>
+      </c>
+      <c r="D46">
+        <v>2.430000005176665</v>
+      </c>
+      <c r="E46">
+        <v>211.2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47">
+        <v>2.41</v>
+      </c>
+      <c r="C47">
+        <v>2.419999280486741</v>
+      </c>
+      <c r="D47">
+        <v>2.43</v>
+      </c>
+      <c r="E47">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48">
+        <v>2.410024510466242</v>
+      </c>
+      <c r="C48">
+        <v>2.419965857391382</v>
+      </c>
+      <c r="D48">
+        <v>2.430001519792279</v>
+      </c>
+      <c r="E48">
+        <v>220.8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49">
+        <v>2.40082237638086</v>
+      </c>
+      <c r="C49">
+        <v>2.421730932154816</v>
+      </c>
+      <c r="D49">
+        <v>2.430393636348344</v>
+      </c>
+      <c r="E49">
+        <v>225.6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50">
+        <v>2.400287438252909</v>
+      </c>
+      <c r="C50">
+        <v>2.409849413183947</v>
+      </c>
+      <c r="D50">
+        <v>2.420169315148204</v>
+      </c>
+      <c r="E50">
+        <v>230.4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51">
+        <v>2.399976290085855</v>
+      </c>
+      <c r="C51">
+        <v>2.410000968719962</v>
+      </c>
+      <c r="D51">
+        <v>2.420000392106276</v>
+      </c>
+      <c r="E51">
+        <v>235.2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52">
         <v>2.4</v>
       </c>
-      <c r="C22">
+      <c r="C52">
         <v>2.41</v>
       </c>
-      <c r="D22">
+      <c r="D52">
         <v>2.42</v>
       </c>
-      <c r="E22">
+      <c r="E52">
         <v>240</v>
       </c>
     </row>

</xml_diff>